<commit_message>
added 2 excel files to tab 2
</commit_message>
<xml_diff>
--- a/Cancer_biobanks_USA.xlsx
+++ b/Cancer_biobanks_USA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vetdd\Documents\PostGrad_NSS\MMCCCL_supply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FE85F0-D232-4E12-8FED-31BCB5A3F9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D8C88A-9EE1-4B65-86CB-887B29C034D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E8EFDF84-A54D-4AED-98AB-682DAEF6A83F}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -28,195 +28,89 @@
     <t xml:space="preserve">contacted </t>
   </si>
   <si>
-    <t>Website</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
     <t>BioIVT (Asterand)</t>
   </si>
   <si>
-    <t>https://www.bioivt.com</t>
-  </si>
-  <si>
-    <t>E customerservice@bioivt.com, 1-516-483-1196</t>
-  </si>
-  <si>
     <t>pending stock check</t>
   </si>
   <si>
     <t>iSpecimen</t>
   </si>
   <si>
-    <t>https://www.ispecimen.com</t>
-  </si>
-  <si>
     <t>Cureline</t>
   </si>
   <si>
-    <t>https://www.cureline.com</t>
-  </si>
-  <si>
-    <t>info@cureline.com, 6507508700</t>
-  </si>
-  <si>
     <t>ProteoGenex</t>
   </si>
   <si>
-    <t>https://www.proteogenex.com</t>
-  </si>
-  <si>
-    <t>support@proteogenex.com, 310 641 0001</t>
-  </si>
-  <si>
     <t>TriStar Group / TriStar Tissue</t>
   </si>
   <si>
-    <t>https://tristargroup.us</t>
-  </si>
-  <si>
-    <t>info@tristargroup.us, 1 866 851 7827</t>
-  </si>
-  <si>
     <t>No tissues are available</t>
   </si>
   <si>
     <t>Conversant Bio</t>
   </si>
   <si>
-    <t>https://www.conversantbio.com</t>
-  </si>
-  <si>
-    <t>Luke Doiron, luke.doiron@conversantbio.com, ph 256-705-6001</t>
-  </si>
-  <si>
     <t>Cooperative Human Tissue Network (CHTN)</t>
   </si>
   <si>
-    <t>https://chtn.org</t>
-  </si>
-  <si>
-    <t>Kradin@chtn.org, 1-317-620-1026, Rebecca Blackwell &lt;rrb5x@uvahealth.org&gt;</t>
-  </si>
-  <si>
     <t>National Disease Research Interchange (NDRI)</t>
   </si>
   <si>
-    <t>https://ndriresource.org</t>
-  </si>
-  <si>
-    <t>research@ndriresource.org, 800 222 6374 ext 3</t>
-  </si>
-  <si>
     <t>MD Anderson Institutional Tissue Bank</t>
   </si>
   <si>
     <t>Memorial Sloan Kettering (MSK) Biobank</t>
   </si>
   <si>
-    <t>https://www.mskcc.org/research/ski/core-facilities/pathology</t>
-  </si>
-  <si>
-    <t>marianom@mskcc.org (lab manager), Joachim Silber director, SilberJ@mskcc.org, ph 646-888-3198</t>
-  </si>
-  <si>
     <t>Dana-Farber / Harvard-affiliated biobank</t>
   </si>
   <si>
-    <t>https://www.dana-farber.org</t>
-  </si>
-  <si>
-    <t>Sujata Shah, ph. 617-582-7441, email: sujata_shah@dfci.harvard.edu</t>
-  </si>
-  <si>
     <t>Johns Hopkins Biobank</t>
   </si>
   <si>
-    <t>https://grcf.jhmi.edu/service/johns-hopkins-biobank/</t>
-  </si>
-  <si>
-    <t>jhbiobank@jhmi.edu, 410-955-3320, 410-614-5201</t>
-  </si>
-  <si>
     <t>Cleveland Clinic Biorepository</t>
   </si>
   <si>
-    <t>https://my.clevelandclinic.org</t>
-  </si>
-  <si>
-    <t>CCBioR@ccf.org</t>
-  </si>
-  <si>
     <t>Stanford Tissue Bank / Cancer Institute Biobank</t>
   </si>
   <si>
-    <t>https://med.stanford.edu/cancer/research/shared-resources/tissue-procurement.html</t>
-  </si>
-  <si>
-    <t>Danielle Leuenberger, dleu@stanford.edu, ph. 650-724-9121</t>
-  </si>
-  <si>
     <t>Biochain</t>
   </si>
   <si>
-    <t>https://www.biochain.com/</t>
-  </si>
-  <si>
-    <t>Rikita Gakhar&lt;rgakhar@biochain.cRom&gt; Ph (O): (510) 783 8588
-cell phone (P): 407-961-8225 (8am to 5:30pm PST)</t>
-  </si>
-  <si>
     <t>reprocell</t>
   </si>
   <si>
-    <t>https://www.reprocell.com/</t>
-  </si>
-  <si>
-    <t>Eric Paz, epaz@reprocellusa.com</t>
-  </si>
-  <si>
     <t>Karmanos cancer institute Wayne State university Biobanking and Correlative Sciences Core</t>
   </si>
   <si>
-    <t>https://www.karmanos.org/karmanos/biobanking-and-correlative-sciences-core</t>
-  </si>
-  <si>
-    <t>Anna Bernard, boernerj@karmanos.org</t>
-  </si>
-  <si>
-    <t>Gray Stowe, gstowe@ispecimen.com</t>
-  </si>
-  <si>
-    <t>tissuebank@mdanderson.org</t>
-  </si>
-  <si>
-    <t>https://www.mdanderson.org/research/research-resources/core-facilities/institutional-tissue-bank.html</t>
-  </si>
-  <si>
     <t>Vantage Biobanking</t>
   </si>
   <si>
-    <t>https://www.vumc.org/vantage/biobanking</t>
-  </si>
-  <si>
     <t>waiting for reply</t>
   </si>
   <si>
-    <t>Contact person</t>
-  </si>
-  <si>
     <t>just storageservice not distributing samples</t>
   </si>
   <si>
-    <t>paxton.g.baker@vumc.org, Baker Paxton G</t>
+    <t>Following the stock check with the CHTN divisions, only one division reported having a few banked cases available. These are likely from the non–African American (non-AA) group. No additional divisions currently have matching tumor FFPE blocks and frozen tissues with corresponding normal adjacent tissue (NAT) available.</t>
+  </si>
+  <si>
+    <t>sent a list of breast tissue 10/29/2025. do not have matched FFPE+FF. We also do not have any black TNBC donors</t>
+  </si>
+  <si>
+    <t>sent an attached samples are in stock and ready to be shipped</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,14 +241,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -683,7 +569,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -726,9 +612,8 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -738,14 +623,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="distributed"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="distributed"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -779,7 +665,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1120,23 +1005,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0ED32E-12DB-4EF7-B094-E29D2C3B4A31}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="75.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="82.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1146,343 +1029,224 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>45952</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="B3" s="4">
         <v>45953</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4">
         <v>45953</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4">
         <v>45953</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
         <v>45952</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4">
         <v>45953</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B8" s="4">
         <v>45952</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4">
         <v>45953</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4">
         <v>45953</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4">
         <v>45953</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B12" s="4">
         <v>45953</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B13" s="4">
         <v>45953</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B14" s="4">
         <v>45953</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4">
         <v>45953</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B16" s="4">
         <v>45952</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B17" s="4">
         <v>45953</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="B18" s="4">
         <v>45953</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>57</v>
+      <c r="C18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="B19" s="4">
         <v>45954</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="3"/>
+      <c r="C19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1" xr:uid="{DEDF73F8-0AFE-4C97-AE9F-CB493EC48F53}"/>
-    <hyperlink ref="C10" r:id="rId2" xr:uid="{3E5E447D-2381-4899-8F5E-DE71EE80A867}"/>
-    <hyperlink ref="D19" r:id="rId3" xr:uid="{A19EE3D1-D0F6-4AE9-8EE0-D06B9DEE2CC8}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>